<commit_message>
add working bulk parser
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="School Data" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,48 +466,593 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Brian's Sample School ES</t>
+          <t>ACPA ES</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C2" t="n">
         <v>2</v>
       </c>
+      <c r="D2" t="n">
+        <v>4</v>
+      </c>
       <c r="E2" t="n">
         <v>1</v>
       </c>
-      <c r="G2" t="n">
-        <v>3</v>
-      </c>
       <c r="H2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Brian's Sample School HS</t>
+          <t>ACPA HS</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D3" t="n">
+        <v>4</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Canton Harbor High School</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>30</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Cascade Career Prep High School</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>30</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Columbus Humanities Arts and Technol</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>46</v>
+      </c>
+      <c r="C6" t="n">
+        <v>3</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Columbus Performance Academy Shepard</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>48</v>
+      </c>
+      <c r="C7" t="n">
+        <v>4</v>
+      </c>
+      <c r="E7" t="n">
         <v>5</v>
       </c>
-      <c r="F3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" t="n">
+      <c r="G7" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Columbus Preparatory Academy ES</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Columbus Preparatory Academy HS</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Columbus Preparatory and Fitness Academy ES</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>63</v>
+      </c>
+      <c r="C10" t="n">
+        <v>5</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Columbus Preparatory and Fitness Academy HS</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>8</v>
+      </c>
+      <c r="C11" t="n">
+        <v>5</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Dayton SMART Elementary School</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>15</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Eastland Performance Academy</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>52</v>
+      </c>
+      <c r="C13" t="n">
+        <v>45</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Fairfield Preparatory Academy</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>35</v>
+      </c>
+      <c r="C14" t="n">
+        <v>2</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Foundation Academy</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>94</v>
+      </c>
+      <c r="C15" t="n">
+        <v>6</v>
+      </c>
+      <c r="D15" t="n">
+        <v>2</v>
+      </c>
+      <c r="E15" t="n">
         <v>3</v>
       </c>
-      <c r="H3" t="n">
-        <v>2</v>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Legacy Academy of Excellence</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>17</v>
+      </c>
+      <c r="C16" t="n">
+        <v>3</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Middletown Preparatory and Fitness Academy</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>78</v>
+      </c>
+      <c r="C17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Mt. Healthy Preparatory and Fitness</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>50</v>
+      </c>
+      <c r="C18" t="n">
+        <v>3</v>
+      </c>
+      <c r="E18" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Northland Preparatory and Fitness Academy</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>24</v>
+      </c>
+      <c r="C19" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Ohio Connections Academy ES</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>526</v>
+      </c>
+      <c r="C20" t="n">
+        <v>28</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Ohio Connections Academy HS</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>328</v>
+      </c>
+      <c r="C21" t="n">
+        <v>17</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Ohio Construction Academy</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>29</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1</v>
+      </c>
+      <c r="E22" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Ohio Digital Learning School</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>226</v>
+      </c>
+      <c r="C23" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Ohio Virtual Academy ES</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>1432</v>
+      </c>
+      <c r="C24" t="n">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Ohio Virtual Academy HS</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>1431</v>
+      </c>
+      <c r="C25" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Riverside Academy</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>35</v>
+      </c>
+      <c r="C26" t="n">
+        <v>3</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Skyway Career Prep High School</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>84</v>
+      </c>
+      <c r="C27" t="n">
+        <v>4</v>
+      </c>
+      <c r="E27" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>South Scioto Performance Academy</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>50</v>
+      </c>
+      <c r="C28" t="n">
+        <v>4</v>
+      </c>
+      <c r="E28" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>South Side Academy</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>28</v>
+      </c>
+      <c r="C29" t="n">
+        <v>2</v>
+      </c>
+      <c r="E29" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Springfield Preparatory and Fitness Academy</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>53</v>
+      </c>
+      <c r="C30" t="n">
+        <v>45</v>
+      </c>
+      <c r="D30" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Toledo Preparatory and Fitness Academy</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>59</v>
+      </c>
+      <c r="C31" t="n">
+        <v>4</v>
+      </c>
+      <c r="E31" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Trotwood Preparatory and Fitness Academy</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>54</v>
+      </c>
+      <c r="C32" t="n">
+        <v>4</v>
+      </c>
+      <c r="E32" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Unknown School</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>21</v>
+      </c>
+      <c r="C33" t="n">
+        <v>1</v>
+      </c>
+      <c r="E33" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Western Toledo Preparatory</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>4</v>
+      </c>
+      <c r="C34" t="n">
+        <v>4</v>
+      </c>
+      <c r="D34" t="n">
+        <v>2</v>
+      </c>
+      <c r="E34" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Whitehall Preparatory and Fitness Academy</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>70</v>
+      </c>
+      <c r="C35" t="n">
+        <v>5</v>
+      </c>
+      <c r="E35" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Wildwood Environmental Academy ES</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>63</v>
+      </c>
+      <c r="C36" t="n">
+        <v>6</v>
+      </c>
+      <c r="D36" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Wildwood Environmental Academy HS</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>24</v>
+      </c>
+      <c r="C37" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Wings Academy 1</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>12</v>
+      </c>
+      <c r="C38" t="n">
+        <v>2</v>
+      </c>
+      <c r="D38" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add file versioning and decimal/duplicate number checks
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,39 +466,30 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ACPA ES</t>
+          <t>85</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>23</v>
-      </c>
-      <c r="C2" t="n">
-        <v>2</v>
-      </c>
-      <c r="D2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E2" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" t="n">
-        <v>1</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ACPA HS</t>
+          <t>ACPA ES</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="C3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D3" t="n">
         <v>4</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
       </c>
       <c r="H3" t="n">
         <v>1</v>
@@ -507,130 +498,136 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Canton Harbor High School</t>
+          <t>ACPA HS</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D4" t="n">
+        <v>4</v>
+      </c>
+      <c r="H4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Cascade Career Prep High School</t>
+          <t>Akron Preparatory School</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="C5" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" t="n">
+        <v>11</v>
+      </c>
+      <c r="G5" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Columbus Humanities Arts and Technol</t>
+          <t>Canton College Prep</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" t="n">
-        <v>3</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Columbus Performance Academy Shepard</t>
+          <t>Canton Harbor High School</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="C7" t="n">
-        <v>4</v>
-      </c>
-      <c r="E7" t="n">
-        <v>5</v>
-      </c>
-      <c r="G7" t="n">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Columbus Preparatory Academy ES</t>
-        </is>
+          <t>Cascade Career Prep High School</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Columbus Preparatory Academy HS</t>
-        </is>
+          <t>Columbus Humanities Arts and Technol</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>46</v>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Columbus Preparatory and Fitness Academy ES</t>
+          <t>Columbus Performance Academy Shepard</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="C10" t="n">
+        <v>4</v>
+      </c>
+      <c r="E10" t="n">
         <v>5</v>
       </c>
-      <c r="D10" t="n">
-        <v>1</v>
+      <c r="G10" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Columbus Preparatory and Fitness Academy HS</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>8</v>
+          <t>Columbus Preparatory Academy ES</t>
+        </is>
       </c>
       <c r="C11" t="n">
-        <v>5</v>
-      </c>
-      <c r="D11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Dayton SMART Elementary School</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>15</v>
+          <t>Columbus Preparatory Academy HS</t>
+        </is>
       </c>
       <c r="C12" t="n">
         <v>1</v>
@@ -639,419 +636,579 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Eastland Performance Academy</t>
+          <t>Columbus Preparatory and Fitness Academy ES</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C13" t="n">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="D13" t="n">
         <v>1</v>
-      </c>
-      <c r="E13" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Fairfield Preparatory Academy</t>
+          <t>Columbus Preparatory and Fitness Academy HS</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C14" t="n">
-        <v>2</v>
-      </c>
-      <c r="E14" t="n">
-        <v>1</v>
-      </c>
-      <c r="G14" t="n">
         <v>5</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Foundation Academy</t>
+          <t>Dayton SMART Elementary School</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>94</v>
+        <v>15</v>
       </c>
       <c r="C15" t="n">
-        <v>6</v>
-      </c>
-      <c r="D15" t="n">
-        <v>2</v>
-      </c>
-      <c r="E15" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Legacy Academy of Excellence</t>
+          <t>Eastland Performance Academy</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="C16" t="n">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="D16" t="n">
         <v>1</v>
+      </c>
+      <c r="E16" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Middletown Preparatory and Fitness Academy</t>
+          <t>Fairfield Preparatory Academy</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="C17" t="n">
+        <v>2</v>
+      </c>
+      <c r="E17" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Mt. Healthy Preparatory and Fitness</t>
+          <t>Foundation Academy</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>50</v>
+        <v>94</v>
       </c>
       <c r="C18" t="n">
+        <v>6</v>
+      </c>
+      <c r="D18" t="n">
+        <v>2</v>
+      </c>
+      <c r="E18" t="n">
         <v>3</v>
-      </c>
-      <c r="E18" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Northland Preparatory and Fitness Academy</t>
+          <t>Great River Connections Academy ES</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>24</v>
+        <v>213</v>
       </c>
       <c r="C19" t="n">
-        <v>2</v>
+        <v>14</v>
+      </c>
+      <c r="D19" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Ohio Connections Academy ES</t>
+          <t>Great River Connections Academy HS</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>526</v>
+        <v>220</v>
       </c>
       <c r="C20" t="n">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="D20" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Ohio Connections Academy HS</t>
+          <t>Lake Erie Preparatory School</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>328</v>
+        <v>32</v>
       </c>
       <c r="C21" t="n">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Ohio Construction Academy</t>
+          <t>Legacy Academy of Excellence</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C22" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D22" t="n">
         <v>1</v>
-      </c>
-      <c r="E22" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Ohio Digital Learning School</t>
+          <t>Mater Academy Preparatory</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>226</v>
+        <v>1</v>
       </c>
       <c r="C23" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Ohio Virtual Academy ES</t>
+          <t>Middletown Preparatory and Fitness Academy</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1432</v>
+        <v>78</v>
       </c>
       <c r="C24" t="n">
-        <v>104</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Ohio Virtual Academy HS</t>
+          <t>Mt. Healthy Preparatory and Fitness</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>1431</v>
+        <v>50</v>
       </c>
       <c r="C25" t="n">
-        <v>57</v>
+        <v>3</v>
+      </c>
+      <c r="E25" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Riverside Academy</t>
+          <t>Northland Preparatory and Fitness Academy</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C26" t="n">
-        <v>3</v>
-      </c>
-      <c r="D26" t="n">
-        <v>1</v>
-      </c>
-      <c r="E26" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Skyway Career Prep High School</t>
+          <t>Ohio Connections Academy ES</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>84</v>
+        <v>526</v>
       </c>
       <c r="C27" t="n">
-        <v>4</v>
-      </c>
-      <c r="E27" t="n">
-        <v>3</v>
+        <v>28</v>
+      </c>
+      <c r="D27" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>South Scioto Performance Academy</t>
+          <t>Ohio Connections Academy HS</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>50</v>
+        <v>328</v>
       </c>
       <c r="C28" t="n">
-        <v>4</v>
-      </c>
-      <c r="E28" t="n">
-        <v>2</v>
+        <v>17</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>South Side Academy</t>
+          <t>Ohio Construction Academy</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C29" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Springfield Preparatory and Fitness Academy</t>
+          <t>Ohio Digital Learning School</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>53</v>
+        <v>226</v>
       </c>
       <c r="C30" t="n">
-        <v>45</v>
-      </c>
-      <c r="D30" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Toledo Preparatory and Fitness Academy</t>
+          <t>Ohio Virtual Academy ES</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>59</v>
+        <v>1432</v>
       </c>
       <c r="C31" t="n">
-        <v>4</v>
-      </c>
-      <c r="E31" t="n">
-        <v>1</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Trotwood Preparatory and Fitness Academy</t>
+          <t>Ohio Virtual Academy HS</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>54</v>
+        <v>1431</v>
       </c>
       <c r="C32" t="n">
-        <v>4</v>
-      </c>
-      <c r="E32" t="n">
-        <v>2</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Unknown School</t>
+          <t>Riverside Academy</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C33" t="n">
+        <v>3</v>
+      </c>
+      <c r="D33" t="n">
         <v>1</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Western Toledo Preparatory</t>
+          <t>STEAM Academy of Warrensville</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="C34" t="n">
-        <v>4</v>
-      </c>
-      <c r="D34" t="n">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="E34" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="H34" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Whitehall Preparatory and Fitness Academy</t>
+          <t>Sheffield Academy</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="C35" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E35" t="n">
         <v>1</v>
+      </c>
+      <c r="G35" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Wildwood Environmental Academy ES</t>
+          <t>Skyway Career Prep High School</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="C36" t="n">
-        <v>6</v>
-      </c>
-      <c r="D36" t="n">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="E36" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Wildwood Environmental Academy HS</t>
+          <t>South Scioto Performance Academy</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="C37" t="n">
-        <v>1</v>
-      </c>
-      <c r="D37" t="n">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="E37" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Wings Academy 1</t>
+          <t>South Side Academy</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="C38" t="n">
         <v>2</v>
       </c>
-      <c r="D38" t="n">
+      <c r="E38" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Springfield Preparatory and Fitness Academy</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>53</v>
+      </c>
+      <c r="C39" t="n">
+        <v>45</v>
+      </c>
+      <c r="D39" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>SunBridge Performance Academy</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>55</v>
+      </c>
+      <c r="C40" t="n">
+        <v>4</v>
+      </c>
+      <c r="E40" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>T-Squared Honors Academy North</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>11</v>
+      </c>
+      <c r="C41" t="n">
+        <v>1</v>
+      </c>
+      <c r="E41" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Toledo Preparatory and Fitness Academy</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>59</v>
+      </c>
+      <c r="C42" t="n">
+        <v>4</v>
+      </c>
+      <c r="E42" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Trotwood Preparatory and Fitness Academy</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>54</v>
+      </c>
+      <c r="C43" t="n">
+        <v>4</v>
+      </c>
+      <c r="E43" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Unknown School</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>21</v>
+      </c>
+      <c r="C44" t="n">
+        <v>1</v>
+      </c>
+      <c r="E44" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Western Toledo Preparatory</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>4</v>
+      </c>
+      <c r="C45" t="n">
+        <v>4</v>
+      </c>
+      <c r="D45" t="n">
+        <v>2</v>
+      </c>
+      <c r="E45" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Whitehall Preparatory and Fitness Academy</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>70</v>
+      </c>
+      <c r="C46" t="n">
+        <v>5</v>
+      </c>
+      <c r="E46" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Wildwood Environmental Academy ES</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>63</v>
+      </c>
+      <c r="C47" t="n">
+        <v>6</v>
+      </c>
+      <c r="D47" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Wildwood Environmental Academy HS</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>24</v>
+      </c>
+      <c r="C48" t="n">
+        <v>1</v>
+      </c>
+      <c r="D48" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>